<commit_message>
- add loading of rusentiment and rutweetcorp, update datasets README - add evaluation of rusentiiment and rutweetcorp - move dataset class to separate file
</commit_message>
<xml_diff>
--- a/data/evaluate_results.xlsx
+++ b/data/evaluate_results.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="21">
   <si>
     <t xml:space="preserve">dataset</t>
   </si>
@@ -77,6 +77,12 @@
   </si>
   <si>
     <t xml:space="preserve">sentirueval_tkk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rusentiment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rutweetcorp</t>
   </si>
 </sst>
 </file>
@@ -285,15 +291,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L19"/>
+  <dimension ref="A1:L28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="19.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="6" style="0" width="19.91"/>
@@ -1025,6 +1031,348 @@
         <v>16</v>
       </c>
     </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="2" t="n">
+        <v>0.533225755251045</v>
+      </c>
+      <c r="C20" s="2" t="n">
+        <v>0.592862047640053</v>
+      </c>
+      <c r="D20" s="2" t="n">
+        <v>0.537313432835821</v>
+      </c>
+      <c r="E20" s="2" t="n">
+        <v>0.636</v>
+      </c>
+      <c r="F20" s="2" t="n">
+        <v>0.463414634146341</v>
+      </c>
+      <c r="G20" s="2" t="n">
+        <v>0.712134632418069</v>
+      </c>
+      <c r="H20" s="2" t="n">
+        <v>0.603036876355748</v>
+      </c>
+      <c r="I20" s="0" t="n">
+        <v>189</v>
+      </c>
+      <c r="J20" s="0" t="n">
+        <v>587</v>
+      </c>
+      <c r="K20" s="0" t="n">
+        <v>224</v>
+      </c>
+      <c r="L20" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="2" t="n">
+        <v>0.571727290410426</v>
+      </c>
+      <c r="C21" s="2" t="n">
+        <v>0.665913431702189</v>
+      </c>
+      <c r="D21" s="2" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="E21" s="2" t="n">
+        <v>0.775</v>
+      </c>
+      <c r="F21" s="2" t="n">
+        <v>0.509433962264151</v>
+      </c>
+      <c r="G21" s="2" t="n">
+        <v>0.854285714285714</v>
+      </c>
+      <c r="H21" s="2" t="n">
+        <v>0.634020618556701</v>
+      </c>
+      <c r="I21" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="J21" s="0" t="n">
+        <v>726</v>
+      </c>
+      <c r="K21" s="0" t="n">
+        <v>174</v>
+      </c>
+      <c r="L21" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="2" t="n">
+        <v>0.337668643121079</v>
+      </c>
+      <c r="C22" s="2" t="n">
+        <v>0.225112428747386</v>
+      </c>
+      <c r="D22" s="2" t="n">
+        <v>0.339514978601997</v>
+      </c>
+      <c r="E22" s="2" t="n">
+        <v>0.238</v>
+      </c>
+      <c r="F22" s="2" t="n">
+        <v>0.345707656612529</v>
+      </c>
+      <c r="G22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H22" s="2" t="n">
+        <v>0.32962962962963</v>
+      </c>
+      <c r="I22" s="0" t="n">
+        <v>184</v>
+      </c>
+      <c r="J22" s="0" t="n">
+        <v>598</v>
+      </c>
+      <c r="K22" s="0" t="n">
+        <v>218</v>
+      </c>
+      <c r="L22" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" s="2" t="n">
+        <v>0.254342021614749</v>
+      </c>
+      <c r="C23" s="2" t="n">
+        <v>0.169561347743166</v>
+      </c>
+      <c r="D23" s="2" t="n">
+        <v>0.253386454183267</v>
+      </c>
+      <c r="E23" s="2" t="n">
+        <v>0.159</v>
+      </c>
+      <c r="F23" s="2" t="n">
+        <v>0.227692307692308</v>
+      </c>
+      <c r="G23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H23" s="2" t="n">
+        <v>0.28099173553719</v>
+      </c>
+      <c r="I23" s="0" t="n">
+        <v>85</v>
+      </c>
+      <c r="J23" s="0" t="n">
+        <v>745</v>
+      </c>
+      <c r="K23" s="0" t="n">
+        <v>170</v>
+      </c>
+      <c r="L23" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24" s="6" t="n">
+        <v>0.644455212515575</v>
+      </c>
+      <c r="C24" s="6" t="n">
+        <v>0.679714762818304</v>
+      </c>
+      <c r="D24" s="6" t="n">
+        <v>0.644468313641246</v>
+      </c>
+      <c r="E24" s="6" t="n">
+        <v>0.701</v>
+      </c>
+      <c r="F24" s="6" t="n">
+        <v>0.632258064516129</v>
+      </c>
+      <c r="G24" s="6" t="n">
+        <v>0.75023386342376</v>
+      </c>
+      <c r="H24" s="6" t="n">
+        <v>0.656652360515021</v>
+      </c>
+      <c r="I24" s="5" t="n">
+        <v>195</v>
+      </c>
+      <c r="J24" s="5" t="n">
+        <v>580</v>
+      </c>
+      <c r="K24" s="5" t="n">
+        <v>225</v>
+      </c>
+      <c r="L24" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B25" s="6" t="n">
+        <v>0.702954561872426</v>
+      </c>
+      <c r="C25" s="6" t="n">
+        <v>0.764615437155969</v>
+      </c>
+      <c r="D25" s="6" t="n">
+        <v>0.704507512520868</v>
+      </c>
+      <c r="E25" s="6" t="n">
+        <v>0.833</v>
+      </c>
+      <c r="F25" s="6" t="n">
+        <v>0.697247706422018</v>
+      </c>
+      <c r="G25" s="6" t="n">
+        <v>0.887937187723055</v>
+      </c>
+      <c r="H25" s="6" t="n">
+        <v>0.708661417322835</v>
+      </c>
+      <c r="I25" s="5" t="n">
+        <v>101</v>
+      </c>
+      <c r="J25" s="5" t="n">
+        <v>720</v>
+      </c>
+      <c r="K25" s="5" t="n">
+        <v>179</v>
+      </c>
+      <c r="L25" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B26" s="6" t="n">
+        <v>0.708693599681972</v>
+      </c>
+      <c r="C26" s="6" t="n">
+        <v>0.699160662031267</v>
+      </c>
+      <c r="D26" s="6" t="n">
+        <v>0.737024221453287</v>
+      </c>
+      <c r="E26" s="6" t="n">
+        <v>0.713</v>
+      </c>
+      <c r="F26" s="6" t="n">
+        <v>0.857558139534884</v>
+      </c>
+      <c r="G26" s="6" t="n">
+        <v>0.680094786729858</v>
+      </c>
+      <c r="H26" s="6" t="n">
+        <v>0.55982905982906</v>
+      </c>
+      <c r="I26" s="5" t="n">
+        <v>330</v>
+      </c>
+      <c r="J26" s="5" t="n">
+        <v>352</v>
+      </c>
+      <c r="K26" s="5" t="n">
+        <v>318</v>
+      </c>
+      <c r="L26" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B27" s="2" t="n">
+        <v>0.683858441392601</v>
+      </c>
+      <c r="C27" s="2" t="n">
+        <v>0.455905627595067</v>
+      </c>
+      <c r="D27" s="2" t="n">
+        <v>0.678271308523409</v>
+      </c>
+      <c r="E27" s="2" t="n">
+        <v>0.565</v>
+      </c>
+      <c r="F27" s="2" t="n">
+        <v>0.75130890052356</v>
+      </c>
+      <c r="G27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H27" s="2" t="n">
+        <v>0.616407982261641</v>
+      </c>
+      <c r="I27" s="0" t="n">
+        <v>330</v>
+      </c>
+      <c r="J27" s="0" t="n">
+        <v>334</v>
+      </c>
+      <c r="K27" s="0" t="n">
+        <v>336</v>
+      </c>
+      <c r="L27" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28" s="2" t="n">
+        <v>0.512053707659445</v>
+      </c>
+      <c r="C28" s="2" t="n">
+        <v>0.53936913843963</v>
+      </c>
+      <c r="D28" s="2" t="n">
+        <v>0.532</v>
+      </c>
+      <c r="E28" s="2" t="n">
+        <v>0.563</v>
+      </c>
+      <c r="F28" s="2" t="n">
+        <v>0.665486725663717</v>
+      </c>
+      <c r="G28" s="2" t="n">
+        <v>0.594</v>
+      </c>
+      <c r="H28" s="2" t="n">
+        <v>0.358620689655172</v>
+      </c>
+      <c r="I28" s="0" t="n">
+        <v>354</v>
+      </c>
+      <c r="J28" s="0" t="n">
+        <v>308</v>
+      </c>
+      <c r="K28" s="0" t="n">
+        <v>338</v>
+      </c>
+      <c r="L28" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>